<commit_message>
website and groups added to mental health
</commit_message>
<xml_diff>
--- a/shinyapp/data/mentalhealthres.xlsx
+++ b/shinyapp/data/mentalhealthres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC85A08F-D234-C645-AF3F-450DB2D43926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAEDAAF2-2BA5-0E47-95FA-C4BBE425B0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14040" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="14040" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Family Engagement" sheetId="1" r:id="rId1"/>

</xml_diff>